<commit_message>
Tilpas diagrammer til udskrift
</commit_message>
<xml_diff>
--- a/08 Projekt Management/Risikoanalyse til Fysioapp.xlsx
+++ b/08 Projekt Management/Risikoanalyse til Fysioapp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\OneDrive\IdeaProjects\Foersteaarsprojekt\08 Projekt Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benky\IdeaProjects\Foersteaarsprojekt\08 Projekt Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="8_{70DDA779-F3BA-44FE-B412-8CB771366CC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{59771D52-11E6-4956-BDDD-40C37DB7B834}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07934620-09A6-4F8E-856B-464013E2759A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC5605DF-97FC-4B92-BFD4-91B241BF52EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC5605DF-97FC-4B92-BFD4-91B241BF52EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Risikoanalyse" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -708,23 +710,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A268E45-2C68-46D3-BBCF-61ECFF0370DE}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="64.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -750,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -778,7 +780,7 @@
         <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -806,7 +808,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -834,7 +836,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -862,7 +864,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -890,7 +892,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -918,7 +920,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -946,7 +948,7 @@
         <v>1.0499999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -974,7 +976,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1002,7 +1004,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1060,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1079,7 +1081,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1107,7 +1109,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
@@ -1156,7 +1158,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1177,149 +1179,149 @@
       <c r="G17" s="3"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="85" fitToWidth="2" fitToHeight="2" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1334,9 +1336,9 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1344,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>5</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>4</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1368,7 +1370,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1376,7 +1378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>0</v>
       </c>

</xml_diff>